<commit_message>
Evap. Intergration and NoEvap Storage plots Update
</commit_message>
<xml_diff>
--- a/2 - RiverWare Modeling/Hydrology/Existing Model Evap Coeffs.xlsx
+++ b/2 - RiverWare Modeling/Hydrology/Existing Model Evap Coeffs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\WeberBasinVulnerability\WeberBasinVulnerability\2 - RiverWare Modeling\Hydrology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747FE7D6-14F8-46C3-8388-813A2069BA50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538D48FC-87C2-45DE-B8F7-EE074B266471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Run0" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="22">
   <si>
     <t>RES1 Smith And Morehouse.Evaporation Coefficients</t>
   </si>
@@ -97,6 +97,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="m/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -136,20 +140,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -432,766 +462,781 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="true" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" customWidth="1"/>
-    <col min="15" max="15" width="2.28515625" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" customWidth="1"/>
-    <col min="18" max="18" width="25" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="23" customWidth="true"/>
+    <col min="3" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="24.28515625" customWidth="true"/>
+    <col min="5" max="5" width="3" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="22.85546875" customWidth="true"/>
+    <col min="7" max="7" width="3" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="22.85546875" customWidth="true"/>
+    <col min="9" max="9" width="3" bestFit="true" customWidth="true"/>
+    <col min="10" max="10" width="24.7109375" customWidth="true"/>
+    <col min="11" max="11" width="3" bestFit="true" customWidth="true"/>
+    <col min="12" max="12" width="23.28515625" customWidth="true"/>
+    <col min="13" max="13" width="3" bestFit="true" customWidth="true"/>
+    <col min="14" max="14" width="23.7109375" customWidth="true"/>
+    <col min="15" max="15" width="2.28515625" customWidth="true"/>
+    <col min="16" max="16" width="22.85546875" customWidth="true"/>
+    <col min="17" max="17" width="2.7109375" customWidth="true"/>
+    <col min="18" max="18" width="25" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    <row r="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="4">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="4">
-        <v>1.9999999999978566E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="R5">
+        <v>0.019999999999978566</v>
+      </c>
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="L6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="M6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="N6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="4">
-        <v>6.0000000000023569E-2</v>
-      </c>
-      <c r="Q6" s="1" t="s">
+      <c r="P6">
+        <v>0.060000000000023569</v>
+      </c>
+      <c r="Q6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6">
         <v>0.14999999999983923</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>0.14000000000020144</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7">
         <v>0.33000000000034929</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>0.31999999999983281</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8">
         <v>0.55000000000028926</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>0.48000000000018855</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <v>0.58000000000008134</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9">
         <v>0.8099999999996591</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>0.41999999999972565</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10">
         <v>0.70000000000012852</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>0.19999999999978565</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11">
         <v>0.41000000000008785</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
-        <v>3.9999999999957132E-2</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12">
+        <v>0.039999999999957132</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="F12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="J12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="K12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="L12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="M12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="O12" s="1" t="s">
+      <c r="N12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="O12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="4">
-        <v>9.0000000000255043E-2</v>
-      </c>
-      <c r="Q12" s="1" t="s">
+      <c r="P12">
+        <v>0.090000000000255043</v>
+      </c>
+      <c r="Q12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12">
         <v>0.17999999999963132</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="4">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1" t="s">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="4">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="4">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="4">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1" t="s">
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1" t="s">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="R14" s="4">
-        <v>0</v>
-      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="T1"/>
     <mergeCell ref="L1"/>
     <mergeCell ref="N1"/>
     <mergeCell ref="P1"/>

</xml_diff>

<commit_message>
Evaporation and Demand updates
</commit_message>
<xml_diff>
--- a/2 - RiverWare Modeling/Hydrology/Existing Model Evap Coeffs.xlsx
+++ b/2 - RiverWare Modeling/Hydrology/Existing Model Evap Coeffs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="22">
   <si>
     <t>RES1 Smith And Morehouse.Evaporation Coefficients</t>
   </si>
@@ -118,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -154,11 +154,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -180,6 +187,15 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -551,55 +567,55 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="R3">
@@ -608,55 +624,55 @@
       <c r="S3" s="2"/>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="R4">
@@ -665,55 +681,55 @@
       <c r="S4" s="2"/>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="Q5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="R5">
@@ -722,55 +738,55 @@
       <c r="S5" s="2"/>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="H6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="J6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="L6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="N6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="P6">
         <v>0.060000000000023569</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" s="18" t="s">
         <v>5</v>
       </c>
       <c r="R6">
@@ -779,55 +795,55 @@
       <c r="S6" s="2"/>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>0.14000000000020144</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="D7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="F7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="H7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="J7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="L7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="N7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="P7">
         <v>0.19999999999978565</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="Q7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="R7">
@@ -836,55 +852,55 @@
       <c r="S7" s="2"/>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>0.31999999999983281</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="F8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="H8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="N8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="P8">
         <v>0.38999999999993351</v>
       </c>
-      <c r="Q8" s="11" t="s">
+      <c r="Q8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="R8">
@@ -893,55 +909,55 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0.48000000000018855</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F9">
         <v>0.58000000000008134</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="H9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="J9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="L9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="N9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="P9">
         <v>0.58999999999971908</v>
       </c>
-      <c r="Q9" s="11" t="s">
+      <c r="Q9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="R9">
@@ -950,55 +966,55 @@
       <c r="S9" s="2"/>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>0.41999999999972565</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="F10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="H10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="J10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="L10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="N10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="O10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="P10">
         <v>0.50999999999998069</v>
       </c>
-      <c r="Q10" s="11" t="s">
+      <c r="Q10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="R10">
@@ -1007,55 +1023,55 @@
       <c r="S10" s="2"/>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>0.19999999999978565</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="H11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="L11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="N11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="O11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="P11">
         <v>0.26999999999988639</v>
       </c>
-      <c r="Q11" s="11" t="s">
+      <c r="Q11" s="18" t="s">
         <v>10</v>
       </c>
       <c r="R11">
@@ -1064,55 +1080,55 @@
       <c r="S11" s="2"/>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>0.039999999999957132</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="J12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="L12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="N12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="P12">
         <v>0.090000000000255043</v>
       </c>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="R12">
@@ -1121,55 +1137,55 @@
       <c r="S12" s="2"/>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13" s="11" t="s">
+      <c r="Q13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="R13">
@@ -1178,55 +1194,55 @@
       <c r="S13" s="2"/>
     </row>
     <row r="14" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="O14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="P14">
         <v>0</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="Q14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="R14">

</xml_diff>